<commit_message>
feat: added the zip of the final submission
</commit_message>
<xml_diff>
--- a/resultados_final.xlsx
+++ b/resultados_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Trepa Colinas" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Evolutivo" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Folha1" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Hibrido" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -852,6 +852,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -874,10 +878,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1044,7 +1044,7 @@
   </sheetPr>
   <dimension ref="A1:L938"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2721,10 +2721,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q202"/>
+  <dimension ref="A1:Q203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N189" activeCellId="0" sqref="N189"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H203" activeCellId="0" sqref="H203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7364,512 +7364,69 @@
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O159" s="12"/>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C160" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D160" s="70" t="n">
-        <v>20</v>
-      </c>
-      <c r="E160" s="70" t="n">
-        <v>20</v>
-      </c>
-      <c r="F160" s="70" t="n">
-        <v>20</v>
-      </c>
-      <c r="G160" s="70" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C161" s="70"/>
-      <c r="D161" s="70"/>
-      <c r="E161" s="70"/>
-      <c r="F161" s="70"/>
-      <c r="G161" s="70"/>
-    </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C162" s="72"/>
-      <c r="D162" s="73"/>
-      <c r="E162" s="73"/>
-      <c r="F162" s="73"/>
-      <c r="G162" s="73"/>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C163" s="72"/>
-      <c r="D163" s="73"/>
-      <c r="E163" s="73"/>
-      <c r="F163" s="73"/>
-      <c r="G163" s="73"/>
-    </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="75"/>
-      <c r="C166" s="76"/>
-      <c r="D166" s="75"/>
-      <c r="E166" s="75"/>
-      <c r="F166" s="75"/>
-      <c r="G166" s="75"/>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="75"/>
-      <c r="C167" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="D167" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="E167" s="77"/>
-      <c r="F167" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="G167" s="77"/>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="C168" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D168" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="E168" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F168" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="G168" s="81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C169" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D169" s="70" t="n">
-        <v>15</v>
-      </c>
-      <c r="E169" s="70" t="n">
-        <v>15</v>
-      </c>
-      <c r="F169" s="70" t="n">
-        <v>15</v>
-      </c>
-      <c r="G169" s="70" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C170" s="70"/>
-      <c r="D170" s="70"/>
-      <c r="E170" s="70"/>
-      <c r="F170" s="70"/>
-      <c r="G170" s="70"/>
-    </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C171" s="72"/>
-      <c r="D171" s="73"/>
-      <c r="E171" s="73"/>
-      <c r="F171" s="73"/>
-      <c r="G171" s="73"/>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C172" s="72"/>
-      <c r="D172" s="73"/>
-      <c r="E172" s="73"/>
-      <c r="F172" s="73"/>
-      <c r="G172" s="73"/>
-    </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="75"/>
-      <c r="C175" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="D175" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="E175" s="77"/>
-      <c r="F175" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="G175" s="77"/>
-    </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="C176" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D176" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="E176" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F176" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="G176" s="81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C177" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D177" s="70" t="n">
-        <v>112</v>
-      </c>
-      <c r="E177" s="82" t="n">
-        <v>110.6</v>
-      </c>
-      <c r="F177" s="70" t="n">
-        <v>112</v>
-      </c>
-      <c r="G177" s="70" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C178" s="70"/>
-      <c r="D178" s="70"/>
-      <c r="E178" s="82"/>
-      <c r="F178" s="70"/>
-      <c r="G178" s="70"/>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C179" s="72"/>
-      <c r="D179" s="73"/>
-      <c r="E179" s="73"/>
-      <c r="F179" s="73"/>
-      <c r="G179" s="73"/>
-    </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C180" s="72"/>
-      <c r="D180" s="73"/>
-      <c r="E180" s="73"/>
-      <c r="F180" s="73"/>
-      <c r="G180" s="73"/>
-    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="75"/>
-      <c r="C182" s="76"/>
-      <c r="D182" s="75"/>
-      <c r="E182" s="75"/>
-      <c r="F182" s="75"/>
-      <c r="G182" s="75"/>
-      <c r="I182" s="75"/>
-      <c r="J182" s="75"/>
+      <c r="I182" s="69"/>
+      <c r="J182" s="69"/>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="75"/>
-      <c r="C183" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="D183" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="E183" s="77"/>
-      <c r="F183" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="G183" s="77"/>
-      <c r="I183" s="75"/>
-      <c r="J183" s="75"/>
+      <c r="I183" s="69"/>
+      <c r="J183" s="69"/>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="C184" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D184" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="E184" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F184" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="G184" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="I184" s="75"/>
-      <c r="J184" s="75"/>
+      <c r="I184" s="69"/>
+      <c r="J184" s="69"/>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C185" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D185" s="70" t="n">
-        <v>79</v>
-      </c>
-      <c r="E185" s="84" t="n">
-        <v>76.139</v>
-      </c>
-      <c r="F185" s="70" t="n">
-        <v>79</v>
-      </c>
-      <c r="G185" s="70" t="n">
-        <v>79</v>
-      </c>
-      <c r="I185" s="75"/>
-      <c r="J185" s="75"/>
-    </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C186" s="70"/>
-      <c r="D186" s="70"/>
-      <c r="E186" s="84"/>
-      <c r="F186" s="70"/>
-      <c r="G186" s="70"/>
-    </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C187" s="72"/>
-      <c r="D187" s="73"/>
-      <c r="E187" s="73"/>
-      <c r="F187" s="73"/>
-      <c r="G187" s="73"/>
-    </row>
+      <c r="I185" s="69"/>
+      <c r="J185" s="69"/>
+    </row>
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C188" s="72"/>
-      <c r="D188" s="73"/>
-      <c r="E188" s="73"/>
-      <c r="F188" s="73"/>
-      <c r="G188" s="73"/>
       <c r="J188" s="12"/>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F190" s="12"/>
-    </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="75"/>
-      <c r="C191" s="76"/>
-      <c r="D191" s="75"/>
-      <c r="E191" s="75"/>
-      <c r="F191" s="75"/>
-      <c r="G191" s="75"/>
-    </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="75"/>
-      <c r="C192" s="83"/>
-      <c r="D192" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="E192" s="85"/>
-      <c r="F192" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="G192" s="85"/>
-    </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="C193" s="87" t="s">
-        <v>64</v>
-      </c>
-      <c r="D193" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="E193" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="F193" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="G193" s="89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="C194" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="D194" s="90" t="n">
-        <v>20</v>
-      </c>
-      <c r="E194" s="91" t="n">
-        <v>20</v>
-      </c>
-      <c r="F194" s="90" t="n">
-        <v>20</v>
-      </c>
-      <c r="G194" s="92" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="71"/>
-      <c r="C195" s="70"/>
-      <c r="D195" s="90"/>
-      <c r="E195" s="91"/>
-      <c r="F195" s="90"/>
-      <c r="G195" s="92"/>
-    </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="C196" s="93" t="s">
-        <v>67</v>
-      </c>
-      <c r="D196" s="94" t="n">
-        <v>15</v>
-      </c>
-      <c r="E196" s="95" t="n">
-        <v>15</v>
-      </c>
-      <c r="F196" s="94" t="n">
-        <v>15</v>
-      </c>
-      <c r="G196" s="95" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="C197" s="93" t="s">
-        <v>69</v>
-      </c>
-      <c r="D197" s="94" t="n">
-        <v>112</v>
-      </c>
-      <c r="E197" s="95" t="n">
-        <v>110.6</v>
-      </c>
-      <c r="F197" s="94" t="n">
-        <v>112</v>
-      </c>
-      <c r="G197" s="95" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C198" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="D198" s="94" t="n">
-        <v>79</v>
-      </c>
-      <c r="E198" s="95" t="n">
-        <v>76.139</v>
-      </c>
-      <c r="F198" s="94" t="n">
-        <v>79</v>
-      </c>
-      <c r="G198" s="95" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="C199" s="96" t="s">
-        <v>71</v>
-      </c>
-      <c r="D199" s="94" t="n">
-        <v>98</v>
-      </c>
-      <c r="E199" s="95" t="n">
-        <v>89.9</v>
-      </c>
-      <c r="F199" s="94" t="n">
-        <v>98</v>
-      </c>
-      <c r="G199" s="95" t="n">
-        <v>96.9</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="71"/>
-      <c r="C200" s="72"/>
-      <c r="D200" s="73"/>
-      <c r="E200" s="73"/>
-      <c r="F200" s="73"/>
-      <c r="G200" s="73"/>
-    </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="74"/>
-      <c r="C201" s="72"/>
-      <c r="D201" s="73"/>
-      <c r="E201" s="73"/>
-      <c r="F201" s="73"/>
-      <c r="G201" s="73"/>
-    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C202" s="75"/>
-      <c r="D202" s="76"/>
-      <c r="E202" s="75"/>
-      <c r="F202" s="75"/>
-      <c r="G202" s="75"/>
-      <c r="H202" s="75"/>
-      <c r="I202" s="75"/>
-      <c r="J202" s="75"/>
-    </row>
+      <c r="I202" s="69"/>
+      <c r="J202" s="69"/>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="139">
+  <mergeCells count="81">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -7951,64 +7508,6 @@
     <mergeCell ref="N145:O145"/>
     <mergeCell ref="B150:B153"/>
     <mergeCell ref="B154:B156"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="G160:G161"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="G162:G163"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="D169:D170"/>
-    <mergeCell ref="E169:E170"/>
-    <mergeCell ref="F169:F170"/>
-    <mergeCell ref="G169:G170"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="D171:D172"/>
-    <mergeCell ref="E171:E172"/>
-    <mergeCell ref="F171:F172"/>
-    <mergeCell ref="G171:G172"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="F175:G175"/>
-    <mergeCell ref="C177:C178"/>
-    <mergeCell ref="D177:D178"/>
-    <mergeCell ref="E177:E178"/>
-    <mergeCell ref="F177:F178"/>
-    <mergeCell ref="G177:G178"/>
-    <mergeCell ref="C179:C180"/>
-    <mergeCell ref="D179:D180"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="G179:G180"/>
-    <mergeCell ref="D183:E183"/>
-    <mergeCell ref="F183:G183"/>
-    <mergeCell ref="C185:C186"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="G185:G186"/>
-    <mergeCell ref="C187:C188"/>
-    <mergeCell ref="D187:D188"/>
-    <mergeCell ref="E187:E188"/>
-    <mergeCell ref="F187:F188"/>
-    <mergeCell ref="G187:G188"/>
-    <mergeCell ref="D192:E192"/>
-    <mergeCell ref="F192:G192"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="D194:D195"/>
-    <mergeCell ref="E194:E195"/>
-    <mergeCell ref="F194:F195"/>
-    <mergeCell ref="G194:G195"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="D200:D201"/>
-    <mergeCell ref="E200:E201"/>
-    <mergeCell ref="F200:F201"/>
-    <mergeCell ref="G200:G201"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8025,14 +7524,572 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="C9:I51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.27"/>
+  </cols>
+  <sheetData>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="71" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" s="71" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="71" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="71" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="73"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="69"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+    </row>
+    <row r="16" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C16" s="69"/>
+      <c r="D16" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="77"/>
+    </row>
+    <row r="17" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="71" t="n">
+        <v>15</v>
+      </c>
+      <c r="F18" s="71" t="n">
+        <v>15</v>
+      </c>
+      <c r="G18" s="71" t="n">
+        <v>15</v>
+      </c>
+      <c r="H18" s="71" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+    </row>
+    <row r="24" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C24" s="69"/>
+      <c r="D24" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="77"/>
+    </row>
+    <row r="25" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="71" t="n">
+        <v>112</v>
+      </c>
+      <c r="F26" s="82" t="n">
+        <v>110.6</v>
+      </c>
+      <c r="G26" s="71" t="n">
+        <v>112</v>
+      </c>
+      <c r="H26" s="71" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="69"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+    </row>
+    <row r="32" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C32" s="69"/>
+      <c r="D32" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="77"/>
+    </row>
+    <row r="33" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="71" t="n">
+        <v>79</v>
+      </c>
+      <c r="F34" s="84" t="n">
+        <v>76.139</v>
+      </c>
+      <c r="G34" s="71" t="n">
+        <v>79</v>
+      </c>
+      <c r="H34" s="71" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="73"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="69"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C41" s="69"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" s="85"/>
+    </row>
+    <row r="42" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="90" t="n">
+        <v>20</v>
+      </c>
+      <c r="F43" s="91" t="n">
+        <v>20</v>
+      </c>
+      <c r="G43" s="90" t="n">
+        <v>20</v>
+      </c>
+      <c r="H43" s="92" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="72"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="92"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="93" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="94" t="n">
+        <v>15</v>
+      </c>
+      <c r="F45" s="95" t="n">
+        <v>15</v>
+      </c>
+      <c r="G45" s="94" t="n">
+        <v>15</v>
+      </c>
+      <c r="H45" s="95" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="94" t="n">
+        <v>112</v>
+      </c>
+      <c r="F46" s="95" t="n">
+        <v>110.6</v>
+      </c>
+      <c r="G46" s="94" t="n">
+        <v>112</v>
+      </c>
+      <c r="H46" s="95" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="94" t="n">
+        <v>79</v>
+      </c>
+      <c r="F47" s="95" t="n">
+        <v>76.139</v>
+      </c>
+      <c r="G47" s="94" t="n">
+        <v>79</v>
+      </c>
+      <c r="H47" s="95" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="96" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="94" t="n">
+        <v>98</v>
+      </c>
+      <c r="F48" s="95" t="n">
+        <v>89.9</v>
+      </c>
+      <c r="G48" s="94" t="n">
+        <v>98</v>
+      </c>
+      <c r="H48" s="95" t="n">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="72"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+    </row>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="75"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="69"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="58">
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>